<commit_message>
small changes to spreadsheet
</commit_message>
<xml_diff>
--- a/Interview Presentation for Candidates - Manchester.xlsx
+++ b/Interview Presentation for Candidates - Manchester.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="1" r:id="rId1"/>
@@ -683,6 +683,16 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -747,16 +757,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1342,11 +1342,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2140875056"/>
-        <c:axId val="-2140871968"/>
+        <c:axId val="-2133681184"/>
+        <c:axId val="-2133678096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2140875056"/>
+        <c:axId val="-2133681184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140871968"/>
+        <c:crossAx val="-2133678096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140871968"/>
+        <c:axId val="-2133678096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140875056"/>
+        <c:crossAx val="-2133681184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2023,11 +2023,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2140782864"/>
-        <c:axId val="-2140779776"/>
+        <c:axId val="-2133616992"/>
+        <c:axId val="-2133613904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2140782864"/>
+        <c:axId val="-2133616992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2070,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140779776"/>
+        <c:crossAx val="-2133613904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2078,7 +2078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140779776"/>
+        <c:axId val="-2133613904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140782864"/>
+        <c:crossAx val="-2133616992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2827,11 +2827,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019010528"/>
-        <c:axId val="-2030926976"/>
+        <c:axId val="-2132615088"/>
+        <c:axId val="-2132611712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019010528"/>
+        <c:axId val="-2132615088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2874,7 +2874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2030926976"/>
+        <c:crossAx val="-2132611712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2882,7 +2882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2030926976"/>
+        <c:axId val="-2132611712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2932,7 +2932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019010528"/>
+        <c:crossAx val="-2132615088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3311,11 +3311,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2083636464"/>
-        <c:axId val="-2063536832"/>
+        <c:axId val="-2132529040"/>
+        <c:axId val="-2132525952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2083636464"/>
+        <c:axId val="-2132529040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063536832"/>
+        <c:crossAx val="-2132525952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3366,7 +3366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2063536832"/>
+        <c:axId val="-2132525952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,7 +3417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083636464"/>
+        <c:crossAx val="-2132529040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3683,11 +3683,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2084830128"/>
-        <c:axId val="-2090856192"/>
+        <c:axId val="-2132483280"/>
+        <c:axId val="-2132480176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2084830128"/>
+        <c:axId val="-2132483280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3730,7 +3730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090856192"/>
+        <c:crossAx val="-2132480176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3738,7 +3738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090856192"/>
+        <c:axId val="-2132480176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3789,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084830128"/>
+        <c:crossAx val="-2132483280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4097,11 +4097,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2019927312"/>
-        <c:axId val="-2090975712"/>
+        <c:axId val="-2133533456"/>
+        <c:axId val="-2133530288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2019927312"/>
+        <c:axId val="-2133533456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,7 +4144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090975712"/>
+        <c:crossAx val="-2133530288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4152,7 +4152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2090975712"/>
+        <c:axId val="-2133530288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4203,7 +4203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019927312"/>
+        <c:crossAx val="-2133533456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4527,11 +4527,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2093416464"/>
-        <c:axId val="-2062183600"/>
+        <c:axId val="-2133490768"/>
+        <c:axId val="-2133487600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2093416464"/>
+        <c:axId val="-2133490768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4574,7 +4574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062183600"/>
+        <c:crossAx val="-2133487600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4582,7 +4582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062183600"/>
+        <c:axId val="-2133487600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4633,7 +4633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093416464"/>
+        <c:crossAx val="-2133490768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8527,7 +8527,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9012,7 +9012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
@@ -9053,141 +9053,141 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58"/>
       <c r="S3" s="3"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61"/>
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="61"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="61"/>
       <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="57"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="61"/>
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="61"/>
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="64"/>
       <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
@@ -9208,56 +9208,56 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
       <c r="S12" s="3"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="63"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="67"/>
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="70"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
@@ -9307,76 +9307,76 @@
       <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="58"/>
       <c r="S18" s="3"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="8"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="61"/>
       <c r="S19" s="3"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="61"/>
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="60"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="64"/>
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.15">
@@ -9434,17 +9434,17 @@
         <v>2018</v>
       </c>
       <c r="O23" s="4"/>
-      <c r="P23" s="51" t="s">
+      <c r="P23" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="Q23" s="51" t="s">
+      <c r="Q23" s="55" t="s">
         <v>49</v>
       </c>
       <c r="R23" s="33"/>
       <c r="S23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -9486,8 +9486,8 @@
         <f>N26*0.21</f>
         <v>190.83308025600002</v>
       </c>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
       <c r="R24" s="33"/>
       <c r="S24" s="3"/>
       <c r="U24" s="22"/>
@@ -9498,7 +9498,7 @@
       <c r="Z24" s="22"/>
     </row>
     <row r="25" spans="1:26" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="8" t="s">
         <v>2</v>
       </c>
@@ -9675,7 +9675,7 @@
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="O29" s="46" t="s">
+      <c r="O29" s="50" t="s">
         <v>48</v>
       </c>
       <c r="S29" s="3"/>
@@ -9697,7 +9697,7 @@
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-      <c r="O30" s="47"/>
+      <c r="O30" s="51"/>
       <c r="S30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="12" thickBot="1" x14ac:dyDescent="0.2">
@@ -9735,7 +9735,7 @@
         <v>2019</v>
       </c>
       <c r="N31" s="20"/>
-      <c r="O31" s="48"/>
+      <c r="O31" s="52"/>
       <c r="P31" s="4"/>
       <c r="S31" s="3"/>
     </row>
@@ -11827,40 +11827,40 @@
       <c r="S75" s="3"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="E76" s="70">
-        <f>(E75/D75)-1</f>
+      <c r="E76" s="49">
+        <f t="shared" ref="E76:M76" si="4">(E75/D75)-1</f>
         <v>7.294776476015663E-2</v>
       </c>
-      <c r="F76" s="70">
-        <f>(F75/E75)-1</f>
+      <c r="F76" s="49">
+        <f t="shared" si="4"/>
         <v>5.7469919451118345E-2</v>
       </c>
-      <c r="G76" s="70">
-        <f>(G75/F75)-1</f>
+      <c r="G76" s="49">
+        <f t="shared" si="4"/>
         <v>5.8553070774883809E-2</v>
       </c>
-      <c r="H76" s="70">
-        <f>(H75/G75)-1</f>
+      <c r="H76" s="49">
+        <f t="shared" si="4"/>
         <v>6.5171193396523996E-2</v>
       </c>
-      <c r="I76" s="70">
-        <f>(I75/H75)-1</f>
+      <c r="I76" s="49">
+        <f t="shared" si="4"/>
         <v>5.7850314322827945E-2</v>
       </c>
-      <c r="J76" s="70">
-        <f>(J75/I75)-1</f>
+      <c r="J76" s="49">
+        <f t="shared" si="4"/>
         <v>6.1676991685256644E-2</v>
       </c>
-      <c r="K76" s="70">
-        <f>(K75/J75)-1</f>
+      <c r="K76" s="49">
+        <f t="shared" si="4"/>
         <v>6.1010485022920058E-2</v>
       </c>
-      <c r="L76" s="70">
-        <f>(L75/K75)-1</f>
+      <c r="L76" s="49">
+        <f t="shared" si="4"/>
         <v>6.0821532369472076E-2</v>
       </c>
-      <c r="M76" s="70">
-        <f>(M75/L75)-1</f>
+      <c r="M76" s="49">
+        <f t="shared" si="4"/>
         <v>6.1018507614383211E-2</v>
       </c>
       <c r="S76" s="3"/>
@@ -11903,27 +11903,27 @@
         <v>0.19487555501242415</v>
       </c>
       <c r="E80" s="43">
-        <f t="shared" ref="E80:J80" si="4">E24/E26</f>
+        <f t="shared" ref="E80:J80" si="5">E24/E26</f>
         <v>0.19503144744194043</v>
       </c>
       <c r="F80" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.20056881068131191</v>
       </c>
       <c r="G80" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.20427278612653069</v>
       </c>
       <c r="H80" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.21009618664301793</v>
       </c>
       <c r="I80" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.21720392336999111</v>
       </c>
       <c r="J80" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.21761617118717677</v>
       </c>
       <c r="K80" s="43">
@@ -11940,27 +11940,27 @@
         <v>0.80512444498757585</v>
       </c>
       <c r="E81" s="43">
-        <f t="shared" ref="E81:J81" si="5">E25/E26</f>
+        <f t="shared" ref="E81:J81" si="6">E25/E26</f>
         <v>0.80496855255805955</v>
       </c>
       <c r="F81" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.79943118931868817</v>
       </c>
       <c r="G81" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.79572721387346945</v>
       </c>
       <c r="H81" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.78990381335698201</v>
       </c>
       <c r="I81" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.78279607663000894</v>
       </c>
       <c r="J81" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.7823838288128232</v>
       </c>
       <c r="K81" s="43">
@@ -12090,7 +12090,7 @@
     <col min="14" max="15" width="9.5" style="2" customWidth="1"/>
     <col min="16" max="16" width="8.33203125" style="2" customWidth="1"/>
     <col min="17" max="18" width="8.83203125" style="2"/>
-    <col min="19" max="19" width="12.1640625" style="67" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" style="46" customWidth="1"/>
     <col min="20" max="20" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="8.83203125" style="2"/>
   </cols>
@@ -12119,134 +12119,134 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="61"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="61"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="57"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="61"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="57"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="61"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="61"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="57"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="61"/>
     </row>
     <row r="10" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="64"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B11" s="37"/>
@@ -12265,54 +12265,54 @@
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="63"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="70"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B15" s="7"/>
@@ -12358,73 +12358,73 @@
       <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="58"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="8"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="61"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="61"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="60"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="64"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B22" s="9"/>
@@ -12493,7 +12493,7 @@
       <c r="R23" s="4">
         <v>2018</v>
       </c>
-      <c r="S23" s="68" t="s">
+      <c r="S23" s="47" t="s">
         <v>69</v>
       </c>
       <c r="T23" s="42" t="s">
@@ -12504,7 +12504,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -12568,7 +12568,7 @@
       <c r="Z24" s="22"/>
     </row>
     <row r="25" spans="1:26" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="8" t="s">
         <v>2</v>
       </c>
@@ -12621,7 +12621,7 @@
       </c>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
-      <c r="S25" s="69">
+      <c r="S25" s="48">
         <f>((C26/H26)^(1/5))-1</f>
         <v>-2.6406092938603409E-2</v>
       </c>
@@ -12749,7 +12749,7 @@
         <v>5.0482319344098414E-2</v>
       </c>
       <c r="P27" s="11">
-        <f t="shared" ref="P27:R27" si="3">(P26/O26)-1</f>
+        <f t="shared" ref="P27" si="3">(P26/O26)-1</f>
         <v>5.2542500281873572E-2</v>
       </c>
       <c r="Q27" s="11"/>
@@ -12768,47 +12768,47 @@
         <v>66</v>
       </c>
       <c r="H29" s="43">
-        <f>H24/H26</f>
+        <f t="shared" ref="H29:N29" si="4">H24/H26</f>
         <v>0.19487555501242415</v>
       </c>
       <c r="I29" s="43">
-        <f>I24/I26</f>
+        <f t="shared" si="4"/>
         <v>0.19503144744194043</v>
       </c>
       <c r="J29" s="43">
-        <f>J24/J26</f>
+        <f t="shared" si="4"/>
         <v>0.20056881068131191</v>
       </c>
       <c r="K29" s="43">
-        <f>K24/K26</f>
+        <f t="shared" si="4"/>
         <v>0.20427278612653069</v>
       </c>
       <c r="L29" s="43">
-        <f>L24/L26</f>
+        <f t="shared" si="4"/>
         <v>0.21009618664301793</v>
       </c>
       <c r="M29" s="43">
-        <f>M24/M26</f>
+        <f t="shared" si="4"/>
         <v>0.21720392336999111</v>
       </c>
       <c r="N29" s="43">
-        <f>N24/N26</f>
+        <f t="shared" si="4"/>
         <v>0.21761617118717677</v>
       </c>
       <c r="O29" s="43">
-        <f>SUM(H24:N24)/SUM(H$26:N$26)</f>
+        <f t="shared" ref="O29:R30" si="5">SUM(H24:N24)/SUM(H$26:N$26)</f>
         <v>0.20583213568242606</v>
       </c>
       <c r="P29" s="43">
-        <f>SUM(I24:O24)/SUM(I$26:O$26)</f>
+        <f t="shared" si="5"/>
         <v>0.20803684672798115</v>
       </c>
       <c r="Q29" s="43">
-        <f>SUM(J24:P24)/SUM(J$26:P$26)</f>
+        <f t="shared" si="5"/>
         <v>0.21005657708361691</v>
       </c>
       <c r="R29" s="43">
-        <f>SUM(K24:Q24)/SUM(K$26:Q$26)</f>
+        <f t="shared" si="5"/>
         <v>0.18023166143789457</v>
       </c>
     </row>
@@ -12817,47 +12817,47 @@
         <v>67</v>
       </c>
       <c r="H30" s="43">
-        <f>H25/H26</f>
+        <f t="shared" ref="H30:N30" si="6">H25/H26</f>
         <v>0.80512444498757585</v>
       </c>
       <c r="I30" s="43">
-        <f>I25/I26</f>
+        <f t="shared" si="6"/>
         <v>0.80496855255805955</v>
       </c>
       <c r="J30" s="43">
-        <f>J25/J26</f>
+        <f t="shared" si="6"/>
         <v>0.79943118931868817</v>
       </c>
       <c r="K30" s="43">
-        <f>K25/K26</f>
+        <f t="shared" si="6"/>
         <v>0.79572721387346945</v>
       </c>
       <c r="L30" s="43">
-        <f>L25/L26</f>
+        <f t="shared" si="6"/>
         <v>0.78990381335698201</v>
       </c>
       <c r="M30" s="43">
-        <f>M25/M26</f>
+        <f t="shared" si="6"/>
         <v>0.78279607663000894</v>
       </c>
       <c r="N30" s="43">
-        <f>N25/N26</f>
+        <f t="shared" si="6"/>
         <v>0.7823838288128232</v>
       </c>
       <c r="O30" s="43">
-        <f>SUM(H25:N25)/SUM(H$26:N$26)</f>
+        <f t="shared" si="5"/>
         <v>0.79416786431757391</v>
       </c>
       <c r="P30" s="43">
-        <f>SUM(I25:O25)/SUM(I$26:O$26)</f>
+        <f t="shared" si="5"/>
         <v>0.79196315327201894</v>
       </c>
       <c r="Q30" s="43">
-        <f>SUM(J25:P25)/SUM(J$26:P$26)</f>
+        <f t="shared" si="5"/>
         <v>0.78994342291638309</v>
       </c>
       <c r="R30" s="43">
-        <f>SUM(K25:Q25)/SUM(K$26:Q$26)</f>
+        <f t="shared" si="5"/>
         <v>0.67180823083555752</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with all figures and charts
</commit_message>
<xml_diff>
--- a/Interview Presentation for Candidates - Manchester.xlsx
+++ b/Interview Presentation for Candidates - Manchester.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Presentation" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="73">
   <si>
     <t xml:space="preserve">The airlines industry comprises passenger air transportation, including both scheduled and chartered, but excludes air freight transport. Industry volumes are defined as the total number of revenue passengers enplaned (departures) at all airports within the country or region, excluding transit passengers who arrive and depart on the same flight code. For the US and Canada, transborder passengers departing from either country are considered as part of the international segment. This avoids the double-counting of passengers. </t>
   </si>
@@ -291,6 +291,15 @@
   <si>
     <t>CAGR 2003-2008</t>
   </si>
+  <si>
+    <t>Total from BTS</t>
+  </si>
+  <si>
+    <t>YOY growth</t>
+  </si>
+  <si>
+    <t>BTS/MarketLine</t>
+  </si>
 </sst>
 </file>
 
@@ -521,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -568,8 +577,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -758,8 +781,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="60">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -782,6 +806,13 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -804,6 +835,13 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1342,11 +1380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133681184"/>
-        <c:axId val="-2133678096"/>
+        <c:axId val="-2133067104"/>
+        <c:axId val="-2138617968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133681184"/>
+        <c:axId val="-2133067104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133678096"/>
+        <c:crossAx val="-2138617968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1397,7 +1435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133678096"/>
+        <c:axId val="-2138617968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133681184"/>
+        <c:crossAx val="-2133067104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1902,7 +1940,46 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0376988373228696"/>
+                  <c:y val="0.00312110776864079"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="hr-HR" baseline="0"/>
+                      <a:t>- 3.5135x2 - 21.436x </a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>+ 745.43</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2023,11 +2100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133616992"/>
-        <c:axId val="-2133613904"/>
+        <c:axId val="-2132159504"/>
+        <c:axId val="-2133023696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133616992"/>
+        <c:axId val="-2132159504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133613904"/>
+        <c:crossAx val="-2133023696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2078,7 +2155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133613904"/>
+        <c:axId val="-2133023696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133616992"/>
+        <c:crossAx val="-2132159504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2827,11 +2904,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132615088"/>
-        <c:axId val="-2132611712"/>
+        <c:axId val="-2132100384"/>
+        <c:axId val="-2132097008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132615088"/>
+        <c:axId val="-2132100384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2874,7 +2951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132611712"/>
+        <c:crossAx val="-2132097008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2882,7 +2959,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132611712"/>
+        <c:axId val="-2132097008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2932,7 +3009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132615088"/>
+        <c:crossAx val="-2132100384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3144,53 +3221,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:forward val="2.0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'US Data (scratch)'!$C$23:$R$23</c:f>
@@ -3311,11 +3341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132529040"/>
-        <c:axId val="-2132525952"/>
+        <c:axId val="-2132911920"/>
+        <c:axId val="-2132908832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132529040"/>
+        <c:axId val="-2132911920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3358,7 +3388,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132525952"/>
+        <c:crossAx val="-2132908832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3366,7 +3396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132525952"/>
+        <c:axId val="-2132908832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,7 +3447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132529040"/>
+        <c:crossAx val="-2132911920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3683,11 +3713,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132483280"/>
-        <c:axId val="-2132480176"/>
+        <c:axId val="-2138883040"/>
+        <c:axId val="-2138871600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132483280"/>
+        <c:axId val="-2138883040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3730,7 +3760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132480176"/>
+        <c:crossAx val="-2138871600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3738,7 +3768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132480176"/>
+        <c:axId val="-2138871600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132483280"/>
+        <c:crossAx val="-2138883040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3868,7 +3898,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Projected European Air Passenger Data 2015-2019</a:t>
+              <a:t>Projected European Passenger Volumes 2015-2019</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4025,6 +4055,30 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presentation!$I$31:$M$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2016.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2017.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2018.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2019.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Presentation!$I$74:$M$74</c:f>
@@ -4050,42 +4104,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredCategoryTitle>
-                <c15:cat>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Presentation!$I$31:$M$31</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="5"/>
-                      <c:pt idx="0">
-                        <c:v>2015.0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2016.0</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2017.0</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>2018.0</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>2019.0</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c15:cat>
-              </c15:filteredCategoryTitle>
-            </c:ext>
-          </c:extLst>
+          <c:extLst/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4097,11 +4116,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133533456"/>
-        <c:axId val="-2133530288"/>
+        <c:axId val="-2132007568"/>
+        <c:axId val="-2132004400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133533456"/>
+        <c:axId val="-2132007568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,7 +4163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133530288"/>
+        <c:crossAx val="-2132004400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4152,7 +4171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133530288"/>
+        <c:axId val="-2132004400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4203,7 +4222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133533456"/>
+        <c:crossAx val="-2132007568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4527,11 +4546,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133490768"/>
-        <c:axId val="-2133487600"/>
+        <c:axId val="-2132871488"/>
+        <c:axId val="-2132868320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133490768"/>
+        <c:axId val="-2132871488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4574,7 +4593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133487600"/>
+        <c:crossAx val="-2132868320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4582,7 +4601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133487600"/>
+        <c:axId val="-2132868320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4633,7 +4652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133490768"/>
+        <c:crossAx val="-2132871488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8527,7 +8546,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9012,8 +9031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z87"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="133" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -12076,17 +12095,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Z36"/>
+  <dimension ref="A2:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" zoomScale="150" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:P26"/>
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="2" customWidth="1"/>
-    <col min="3" max="13" width="8.33203125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="8.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="8.33203125" style="2" customWidth="1"/>
     <col min="14" max="15" width="9.5" style="2" customWidth="1"/>
     <col min="16" max="16" width="8.33203125" style="2" customWidth="1"/>
     <col min="17" max="18" width="8.83203125" style="2"/>
@@ -12688,11 +12709,11 @@
         <v>840.17100000000005</v>
       </c>
       <c r="Q26" s="32">
-        <f>($C$32*(Q23-2002))+$D$32</f>
+        <f>($C$35*(Q23-2002))+$D$35</f>
         <v>798.35518710989015</v>
       </c>
       <c r="R26" s="32">
-        <f>($C$32*(R23-2002))+$D$32</f>
+        <f>($C$35*(R23-2002))+$D$35</f>
         <v>806.39382016263744</v>
       </c>
       <c r="T26" s="44"/>
@@ -12704,201 +12725,323 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11">
-        <f t="shared" ref="D27:H27" si="2">(D26/C26)-1</f>
+      <c r="B27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="32">
+        <v>644.23497299999997</v>
+      </c>
+      <c r="D27" s="32">
+        <v>700.230727</v>
+      </c>
+      <c r="E27" s="32">
+        <v>735.10466799999995</v>
+      </c>
+      <c r="F27" s="32">
+        <v>741.09819900000002</v>
+      </c>
+      <c r="G27" s="32">
+        <v>766.62658199999998</v>
+      </c>
+      <c r="H27" s="32">
+        <v>740.46093299999995</v>
+      </c>
+      <c r="I27" s="32">
+        <v>701.16445499999998</v>
+      </c>
+      <c r="J27" s="32">
+        <v>717.744056</v>
+      </c>
+      <c r="K27" s="32">
+        <v>728.36829699999998</v>
+      </c>
+      <c r="L27" s="32">
+        <v>734.32246899999996</v>
+      </c>
+      <c r="M27" s="32">
+        <v>740.85938699999997</v>
+      </c>
+      <c r="N27" s="32">
+        <v>761.00355300000001</v>
+      </c>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="32"/>
+      <c r="T27" s="44"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="22"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A28" s="8"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="71">
+        <f>H27/H26</f>
+        <v>1.0054190028107051</v>
+      </c>
+      <c r="I28" s="71">
+        <f t="shared" ref="I28:N28" si="2">I27/I26</f>
+        <v>1.0045479949569478</v>
+      </c>
+      <c r="J28" s="71">
+        <f t="shared" si="2"/>
+        <v>1.005567698278157</v>
+      </c>
+      <c r="K28" s="71">
+        <f t="shared" si="2"/>
+        <v>1.0032759363076627</v>
+      </c>
+      <c r="L28" s="71">
+        <f t="shared" si="2"/>
+        <v>1.0018725274575344</v>
+      </c>
+      <c r="M28" s="71">
+        <f t="shared" si="2"/>
+        <v>1.0009178672755277</v>
+      </c>
+      <c r="N28" s="71">
+        <f t="shared" si="2"/>
+        <v>1.0014917722768368</v>
+      </c>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="R28" s="32"/>
+      <c r="T28" s="44"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11">
+        <f t="shared" ref="D29:H29" si="3">(D26/C26)-1</f>
         <v>8.6918215164950352E-2</v>
       </c>
-      <c r="E27" s="11">
-        <f t="shared" si="2"/>
+      <c r="E29" s="11">
+        <f t="shared" si="3"/>
         <v>4.980349998265643E-2</v>
       </c>
-      <c r="F27" s="11">
-        <f t="shared" si="2"/>
+      <c r="F29" s="11">
+        <f t="shared" si="3"/>
         <v>8.1533028708777877E-3</v>
       </c>
-      <c r="G27" s="11">
-        <f t="shared" si="2"/>
+      <c r="G29" s="11">
+        <f t="shared" si="3"/>
         <v>3.4446694155304547E-2</v>
       </c>
-      <c r="H27" s="11">
-        <f t="shared" si="2"/>
+      <c r="H29" s="11">
+        <f t="shared" si="3"/>
         <v>-3.9336728869127535E-2</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I29" s="35">
         <v>-5.224924301057754E-2</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J29" s="35">
         <v>2.2607773750340288E-2</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K29" s="35">
         <v>1.7134295882232253E-2</v>
       </c>
-      <c r="L27" s="35">
+      <c r="L29" s="35">
         <v>9.589772929834206E-3</v>
       </c>
-      <c r="M27" s="35">
+      <c r="M29" s="35">
         <v>9.8590614317832781E-3</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N29" s="35">
         <v>2.6594720169837549E-2</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O29" s="11">
         <f>(O26/N26)-1</f>
         <v>5.0482319344098414E-2</v>
       </c>
-      <c r="P27" s="11">
-        <f t="shared" ref="P27" si="3">(P26/O26)-1</f>
+      <c r="P29" s="11">
+        <f t="shared" ref="P29" si="4">(P26/O26)-1</f>
         <v>5.2542500281873572E-2</v>
       </c>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="K28" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" s="43">
-        <f t="shared" ref="H29:N29" si="4">H24/H26</f>
-        <v>0.19487555501242415</v>
-      </c>
-      <c r="I29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.19503144744194043</v>
-      </c>
-      <c r="J29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.20056881068131191</v>
-      </c>
-      <c r="K29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.20427278612653069</v>
-      </c>
-      <c r="L29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.21009618664301793</v>
-      </c>
-      <c r="M29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.21720392336999111</v>
-      </c>
-      <c r="N29" s="43">
-        <f t="shared" si="4"/>
-        <v>0.21761617118717677</v>
-      </c>
-      <c r="O29" s="43">
-        <f t="shared" ref="O29:R30" si="5">SUM(H24:N24)/SUM(H$26:N$26)</f>
-        <v>0.20583213568242606</v>
-      </c>
-      <c r="P29" s="43">
-        <f t="shared" si="5"/>
-        <v>0.20803684672798115</v>
-      </c>
-      <c r="Q29" s="43">
-        <f t="shared" si="5"/>
-        <v>0.21005657708361691</v>
-      </c>
-      <c r="R29" s="43">
-        <f t="shared" si="5"/>
-        <v>0.18023166143789457</v>
-      </c>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="43">
-        <f t="shared" ref="H30:N30" si="6">H25/H26</f>
-        <v>0.80512444498757585</v>
-      </c>
-      <c r="I30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.80496855255805955</v>
-      </c>
-      <c r="J30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.79943118931868817</v>
-      </c>
-      <c r="K30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.79572721387346945</v>
-      </c>
-      <c r="L30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.78990381335698201</v>
-      </c>
-      <c r="M30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.78279607663000894</v>
-      </c>
-      <c r="N30" s="43">
-        <f t="shared" si="6"/>
-        <v>0.7823838288128232</v>
-      </c>
-      <c r="O30" s="43">
-        <f t="shared" si="5"/>
-        <v>0.79416786431757391</v>
-      </c>
-      <c r="P30" s="43">
-        <f t="shared" si="5"/>
-        <v>0.79196315327201894</v>
-      </c>
-      <c r="Q30" s="43">
-        <f t="shared" si="5"/>
-        <v>0.78994342291638309</v>
-      </c>
-      <c r="R30" s="43">
-        <f t="shared" si="5"/>
-        <v>0.67180823083555752</v>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="K31" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="C32" s="2">
-        <f t="array" ref="C32:D36">LINEST(C26:P26,,,TRUE)</f>
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="43">
+        <f t="shared" ref="H32:N32" si="5">H24/H26</f>
+        <v>0.19487555501242415</v>
+      </c>
+      <c r="I32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.19503144744194043</v>
+      </c>
+      <c r="J32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.20056881068131191</v>
+      </c>
+      <c r="K32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.20427278612653069</v>
+      </c>
+      <c r="L32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.21009618664301793</v>
+      </c>
+      <c r="M32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.21720392336999111</v>
+      </c>
+      <c r="N32" s="43">
+        <f t="shared" si="5"/>
+        <v>0.21761617118717677</v>
+      </c>
+      <c r="O32" s="43">
+        <f t="shared" ref="O32:R33" si="6">SUM(H24:N24)/SUM(H$26:N$26)</f>
+        <v>0.20583213568242606</v>
+      </c>
+      <c r="P32" s="43">
+        <f t="shared" si="6"/>
+        <v>0.20803684672798115</v>
+      </c>
+      <c r="Q32" s="43">
+        <f t="shared" si="6"/>
+        <v>0.21005657708361691</v>
+      </c>
+      <c r="R32" s="43">
+        <f t="shared" si="6"/>
+        <v>0.18023166143789457</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="43">
+        <f t="shared" ref="H33:N33" si="7">H25/H26</f>
+        <v>0.80512444498757585</v>
+      </c>
+      <c r="I33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.80496855255805955</v>
+      </c>
+      <c r="J33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.79943118931868817</v>
+      </c>
+      <c r="K33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.79572721387346945</v>
+      </c>
+      <c r="L33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.78990381335698201</v>
+      </c>
+      <c r="M33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.78279607663000894</v>
+      </c>
+      <c r="N33" s="43">
+        <f t="shared" si="7"/>
+        <v>0.7823838288128232</v>
+      </c>
+      <c r="O33" s="43">
+        <f t="shared" si="6"/>
+        <v>0.79416786431757391</v>
+      </c>
+      <c r="P33" s="43">
+        <f t="shared" si="6"/>
+        <v>0.79196315327201894</v>
+      </c>
+      <c r="Q33" s="43">
+        <f t="shared" si="6"/>
+        <v>0.78994342291638309</v>
+      </c>
+      <c r="R33" s="43">
+        <f t="shared" si="6"/>
+        <v>0.67180823083555752</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="C35" s="2">
+        <f t="array" ref="C35:D39">LINEST(C26:P26,,,TRUE)</f>
         <v>8.0386330527472563</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D35" s="2">
         <v>677.77569131868131</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C33" s="2">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="C36" s="2">
         <v>2.2042607245395613</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D36" s="2">
         <v>18.768603764710527</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C34" s="2">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="C37" s="2">
         <v>0.52568414581677692</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D37" s="2">
         <v>33.247091831430836</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C35" s="2">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="C38" s="2">
         <v>13.299597081071909</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D38" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C36" s="2">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="C39" s="2">
         <v>14700.963858653955</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D39" s="2">
         <v>13264.429382971142</v>
       </c>
     </row>

</xml_diff>